<commit_message>
added ignore for cancelled pilots
</commit_message>
<xml_diff>
--- a/calculator.xlsx
+++ b/calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben.woodcock\Documents\Personal\CIVL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben.woodcock\Documents\Personal\CIVL\Civl-Ripper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF321BCA-9AA0-45C5-AADE-7D636E95E8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C256C8-F04C-4B21-A38B-27952A235356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DD4F1E63-7E87-4339-B031-125C2E1D83F3}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="123">
   <si>
     <t>usa</t>
   </si>
@@ -452,11 +452,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -776,16 +773,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF33F86B-7085-48D0-9A19-108071314EB3}">
-  <dimension ref="A1:F176"/>
+  <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="62" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="62" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -798,567 +795,567 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <f>D2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <f t="shared" ref="F3:F66" si="0">D3</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>14</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>16</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>17</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>18</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>19</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>20</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>21</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>22</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24">
         <v>23</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25">
         <v>24</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>25</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>26</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>27</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>28</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30">
         <v>29</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>30</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>31</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -1370,121 +1367,121 @@
       <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>32</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>33</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="3">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>34</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>35</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>36</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38">
         <v>37</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" t="s">
         <v>83</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39">
         <v>38</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
@@ -1494,339 +1491,339 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40">
         <v>39</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" t="s">
         <v>84</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41">
         <v>40</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42">
         <v>41</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" t="s">
         <v>86</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43">
         <v>42</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="3">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44">
         <v>43</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" t="s">
         <v>89</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="3">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45">
         <v>44</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" t="s">
         <v>90</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="3">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46">
         <v>45</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" t="s">
         <v>91</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="3">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47">
         <v>46</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="3">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48">
         <v>47</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" t="s">
         <v>93</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="3">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49">
         <v>48</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" t="s">
         <v>94</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="3">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50">
         <v>49</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50" s="3">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51">
         <v>50</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52">
         <v>51</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" t="s">
         <v>97</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52" s="3">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53">
         <v>52</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" t="s">
         <v>98</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="3">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54">
         <v>53</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" t="s">
         <v>99</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54" s="3">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55">
         <v>54</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" t="s">
         <v>100</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55" s="3">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56">
         <v>55</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" t="s">
         <v>105</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="3">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57">
         <v>56</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" t="s">
         <v>101</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57" s="3">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58">
         <v>57</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" t="s">
         <v>102</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="3">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
@@ -1838,103 +1835,103 @@
       <c r="B59" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59">
         <v>58</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" t="s">
         <v>103</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="3">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60">
         <v>59</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" t="s">
         <v>104</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60" s="3">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61">
         <v>60</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" t="s">
         <v>106</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="3">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62">
         <v>61</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" t="s">
         <v>107</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62" s="3">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
-      </c>
-      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63">
         <v>62</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" t="s">
         <v>108</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="3">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64">
         <v>63</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" t="s">
         <v>109</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="3">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
@@ -1944,256 +1941,256 @@
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65">
         <v>64</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F65" s="3">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66">
         <v>65</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" t="s">
         <v>111</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F66" s="3">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67">
         <v>66</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" t="s">
         <v>112</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67" s="3">
         <f t="shared" ref="F67:F82" si="1">D67</f>
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68">
         <v>67</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" t="s">
         <v>113</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68" s="3">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69">
         <v>68</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" t="s">
         <v>114</v>
       </c>
-      <c r="F69" s="4">
+      <c r="F69" s="3">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
-      </c>
-      <c r="F72" s="4">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>100</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
-      </c>
-      <c r="F74" s="4">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
-      </c>
-      <c r="F75" s="4">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
-      </c>
-      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="F76" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F77" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
       </c>
-      <c r="F78" s="4">
+      <c r="F78" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
       </c>
-      <c r="F79" s="4">
+      <c r="F79" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
       </c>
-      <c r="F80" s="4">
+      <c r="F80" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
       </c>
-      <c r="F81" s="4">
+      <c r="F81" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
@@ -2201,23 +2198,23 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -2225,7 +2222,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
@@ -2233,7 +2230,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -2241,7 +2238,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -2257,23 +2254,23 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
@@ -2281,7 +2278,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B94" t="s">
         <v>1</v>
@@ -2289,7 +2286,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
         <v>1</v>
@@ -2297,7 +2294,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
@@ -2305,7 +2302,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
@@ -2321,7 +2318,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
@@ -2329,7 +2326,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
@@ -2337,7 +2334,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -2345,7 +2342,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B102" t="s">
         <v>1</v>
@@ -2353,7 +2350,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B103" t="s">
         <v>1</v>
@@ -2361,7 +2358,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
@@ -2369,31 +2366,31 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B107" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B108" t="s">
         <v>1</v>
@@ -2401,7 +2398,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B109" t="s">
         <v>1</v>
@@ -2409,7 +2406,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B110" t="s">
         <v>1</v>
@@ -2425,15 +2422,15 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B112" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
         <v>1</v>
@@ -2441,7 +2438,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B114" t="s">
         <v>1</v>
@@ -2449,15 +2446,15 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B115" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B116" t="s">
         <v>1</v>
@@ -2465,7 +2462,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B117" t="s">
         <v>1</v>
@@ -2473,7 +2470,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B118" t="s">
         <v>1</v>
@@ -2481,7 +2478,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B119" t="s">
         <v>1</v>
@@ -2489,23 +2486,23 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B122" t="s">
         <v>1</v>
@@ -2513,7 +2510,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B123" t="s">
         <v>1</v>
@@ -2521,7 +2518,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B124" t="s">
         <v>1</v>
@@ -2529,7 +2526,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B125" t="s">
         <v>1</v>
@@ -2537,7 +2534,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B126" t="s">
         <v>1</v>
@@ -2545,7 +2542,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B127" t="s">
         <v>1</v>
@@ -2553,7 +2550,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B128" t="s">
         <v>1</v>
@@ -2561,7 +2558,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B129" t="s">
         <v>1</v>
@@ -2569,7 +2566,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B130" t="s">
         <v>1</v>
@@ -2577,7 +2574,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B131" t="s">
         <v>1</v>
@@ -2585,7 +2582,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B132" t="s">
         <v>1</v>
@@ -2593,7 +2590,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B133" t="s">
         <v>1</v>
@@ -2601,7 +2598,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B134" t="s">
         <v>1</v>
@@ -2609,7 +2606,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B135" t="s">
         <v>1</v>
@@ -2617,7 +2614,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B136" t="s">
         <v>1</v>
@@ -2625,7 +2622,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B137" t="s">
         <v>1</v>
@@ -2633,7 +2630,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B138" t="s">
         <v>1</v>
@@ -2641,15 +2638,15 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B139" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B140" t="s">
         <v>1</v>
@@ -2657,7 +2654,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B141" t="s">
         <v>1</v>
@@ -2665,15 +2662,15 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B143" t="s">
         <v>40</v>
@@ -2681,74 +2678,74 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B144" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B145" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B146" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B148" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B149" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B150" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B151" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B152" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -2756,12 +2753,12 @@
         <v>27</v>
       </c>
       <c r="B153" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B154" t="s">
         <v>40</v>
@@ -2769,55 +2766,55 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B155" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B156" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B157" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B159" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B160" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B161" t="s">
         <v>40</v>
@@ -2825,66 +2822,66 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B162" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B163" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B165" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B166" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B167" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B168" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B169" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -2897,7 +2894,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B171" t="s">
         <v>40</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B172" t="s">
         <v>40</v>
@@ -2913,34 +2910,66 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B173" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B174" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B175" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B176" t="s">
-        <v>1</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>17</v>
+      </c>
+      <c r="B177" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>33</v>
+      </c>
+      <c r="B178" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>37</v>
+      </c>
+      <c r="B179" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>42</v>
+      </c>
+      <c r="B180" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2962,13 +2991,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="33.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2978,7 +3007,7 @@
       <c r="B1" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D1" t="s">
@@ -3005,7 +3034,7 @@
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D2">
@@ -3017,15 +3046,15 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <f>IF(AND(D2&lt;&gt;0, E2&lt;&gt;0),3,IF(D2+E2&gt;1,2,D2+E2))</f>
+        <f t="shared" ref="F2:F33" si="0">IF(AND(D2&lt;&gt;0, E2&lt;&gt;0),3,IF(D2+E2&gt;1,2,D2+E2))</f>
         <v>2</v>
       </c>
       <c r="G2">
-        <f>IF(F2=E2+D2,0,1)</f>
+        <f t="shared" ref="G2:G33" si="1">IF(F2=E2+D2,0,1)</f>
         <v>1</v>
       </c>
       <c r="H2">
-        <f>IF(G2+F2&lt;E2+D2,1,0)</f>
+        <f t="shared" ref="H2:H33" si="2">IF(G2+F2&lt;E2+D2,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3037,27 +3066,27 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D3">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B3,INPUT!$B:$B,"M")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B3,INPUT!$B:$B,"F")</f>
         <v>1</v>
       </c>
       <c r="F3">
-        <f>IF(AND(D3&lt;&gt;0, E3&lt;&gt;0),3,IF(D3+E3&gt;1,2,D3+E3))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G3">
-        <f>IF(F3=E3+D3,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H3">
-        <f>IF(G3+F3&lt;E3+D3,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3069,7 +3098,7 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D4">
@@ -3081,15 +3110,15 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <f>IF(AND(D4&lt;&gt;0, E4&lt;&gt;0),3,IF(D4+E4&gt;1,2,D4+E4))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G4">
-        <f>IF(F4=E4+D4,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f>IF(G4+F4&lt;E4+D4,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3101,7 +3130,7 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D5">
@@ -3113,15 +3142,15 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f>IF(AND(D5&lt;&gt;0, E5&lt;&gt;0),3,IF(D5+E5&gt;1,2,D5+E5))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G5">
-        <f>IF(F5=E5+D5,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>IF(G5+F5&lt;E5+D5,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3133,7 +3162,7 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D6">
@@ -3145,15 +3174,15 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f>IF(AND(D6&lt;&gt;0, E6&lt;&gt;0),3,IF(D6+E6&gt;1,2,D6+E6))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G6">
-        <f>IF(F6=E6+D6,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H6">
-        <f>IF(G6+F6&lt;E6+D6,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3173,15 +3202,15 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f>IF(AND(D7&lt;&gt;0, E7&lt;&gt;0),3,IF(D7+E7&gt;1,2,D7+E7))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>IF(F7=E7+D7,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>IF(G7+F7&lt;E7+D7,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3193,7 +3222,7 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D8">
@@ -3205,15 +3234,15 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <f>IF(AND(D8&lt;&gt;0, E8&lt;&gt;0),3,IF(D8+E8&gt;1,2,D8+E8))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G8">
-        <f>IF(F8=E8+D8,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H8">
-        <f>IF(G8+F8&lt;E8+D8,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3225,7 +3254,7 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D9">
@@ -3237,15 +3266,15 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <f>IF(AND(D9&lt;&gt;0, E9&lt;&gt;0),3,IF(D9+E9&gt;1,2,D9+E9))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G9">
-        <f>IF(F9=E9+D9,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>IF(G9+F9&lt;E9+D9,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3257,7 +3286,7 @@
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D10">
@@ -3269,15 +3298,15 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <f>IF(AND(D10&lt;&gt;0, E10&lt;&gt;0),3,IF(D10+E10&gt;1,2,D10+E10))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G10">
-        <f>IF(F10=E10+D10,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H10">
-        <f>IF(G10+F10&lt;E10+D10,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3297,15 +3326,15 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <f>IF(AND(D11&lt;&gt;0, E11&lt;&gt;0),3,IF(D11+E11&gt;1,2,D11+E11))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>IF(F11=E11+D11,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f>IF(G11+F11&lt;E11+D11,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3317,7 +3346,7 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D12">
@@ -3326,18 +3355,18 @@
       </c>
       <c r="E12">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B12,INPUT!$B:$B,"F")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <f>IF(AND(D12&lt;&gt;0, E12&lt;&gt;0),3,IF(D12+E12&gt;1,2,D12+E12))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G12">
-        <f>IF(F12=E12+D12,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H12">
-        <f>IF(G12+F12&lt;E12+D12,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3349,7 +3378,7 @@
       <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D13">
@@ -3361,15 +3390,15 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f>IF(AND(D13&lt;&gt;0, E13&lt;&gt;0),3,IF(D13+E13&gt;1,2,D13+E13))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G13">
-        <f>IF(F13=E13+D13,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H13">
-        <f>IF(G13+F13&lt;E13+D13,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3381,7 +3410,7 @@
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D14">
@@ -3393,15 +3422,15 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <f>IF(AND(D14&lt;&gt;0, E14&lt;&gt;0),3,IF(D14+E14&gt;1,2,D14+E14))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G14">
-        <f>IF(F14=E14+D14,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H14">
-        <f>IF(G14+F14&lt;E14+D14,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3421,15 +3450,15 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <f>IF(AND(D15&lt;&gt;0, E15&lt;&gt;0),3,IF(D15+E15&gt;1,2,D15+E15))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>IF(F15=E15+D15,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>IF(G15+F15&lt;E15+D15,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3441,7 +3470,7 @@
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D16">
@@ -3453,15 +3482,15 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <f>IF(AND(D16&lt;&gt;0, E16&lt;&gt;0),3,IF(D16+E16&gt;1,2,D16+E16))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G16">
-        <f>IF(F16=E16+D16,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H16">
-        <f>IF(G16+F16&lt;E16+D16,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3473,7 +3502,7 @@
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D17">
@@ -3485,15 +3514,15 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <f>IF(AND(D17&lt;&gt;0, E17&lt;&gt;0),3,IF(D17+E17&gt;1,2,D17+E17))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G17">
-        <f>IF(F17=E17+D17,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H17">
-        <f>IF(G17+F17&lt;E17+D17,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3505,7 +3534,7 @@
       <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D18">
@@ -3517,15 +3546,15 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <f>IF(AND(D18&lt;&gt;0, E18&lt;&gt;0),3,IF(D18+E18&gt;1,2,D18+E18))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G18">
-        <f>IF(F18=E18+D18,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>IF(G18+F18&lt;E18+D18,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3537,7 +3566,7 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D19">
@@ -3549,15 +3578,15 @@
         <v>5</v>
       </c>
       <c r="F19">
-        <f>IF(AND(D19&lt;&gt;0, E19&lt;&gt;0),3,IF(D19+E19&gt;1,2,D19+E19))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G19">
-        <f>IF(F19=E19+D19,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H19">
-        <f>IF(G19+F19&lt;E19+D19,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3569,7 +3598,7 @@
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D20">
@@ -3581,15 +3610,15 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <f>IF(AND(D20&lt;&gt;0, E20&lt;&gt;0),3,IF(D20+E20&gt;1,2,D20+E20))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G20">
-        <f>IF(F20=E20+D20,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H20">
-        <f>IF(G20+F20&lt;E20+D20,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3601,7 +3630,7 @@
       <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D21">
@@ -3613,15 +3642,15 @@
         <v>3</v>
       </c>
       <c r="F21">
-        <f>IF(AND(D21&lt;&gt;0, E21&lt;&gt;0),3,IF(D21+E21&gt;1,2,D21+E21))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G21">
-        <f>IF(F21=E21+D21,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H21">
-        <f>IF(G21+F21&lt;E21+D21,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3633,7 +3662,7 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D22">
@@ -3645,15 +3674,15 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <f>IF(AND(D22&lt;&gt;0, E22&lt;&gt;0),3,IF(D22+E22&gt;1,2,D22+E22))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G22">
-        <f>IF(F22=E22+D22,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H22">
-        <f>IF(G22+F22&lt;E22+D22,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3665,7 +3694,7 @@
       <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D23">
@@ -3677,15 +3706,15 @@
         <v>3</v>
       </c>
       <c r="F23">
-        <f>IF(AND(D23&lt;&gt;0, E23&lt;&gt;0),3,IF(D23+E23&gt;1,2,D23+E23))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G23">
-        <f>IF(F23=E23+D23,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H23">
-        <f>IF(G23+F23&lt;E23+D23,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3697,7 +3726,7 @@
       <c r="B24" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D24">
@@ -3709,15 +3738,15 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <f>IF(AND(D24&lt;&gt;0, E24&lt;&gt;0),3,IF(D24+E24&gt;1,2,D24+E24))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G24">
-        <f>IF(F24=E24+D24,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H24">
-        <f>IF(G24+F24&lt;E24+D24,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3729,7 +3758,7 @@
       <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D25">
@@ -3741,15 +3770,15 @@
         <v>3</v>
       </c>
       <c r="F25">
-        <f>IF(AND(D25&lt;&gt;0, E25&lt;&gt;0),3,IF(D25+E25&gt;1,2,D25+E25))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G25">
-        <f>IF(F25=E25+D25,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H25">
-        <f>IF(G25+F25&lt;E25+D25,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3761,27 +3790,27 @@
       <c r="B26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D26">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B25,INPUT!$B:$B,"M")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B25,INPUT!$B:$B,"F")</f>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>IF(AND(D26&lt;&gt;0, E26&lt;&gt;0),3,IF(D26+E26&gt;1,2,D26+E26))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G26">
-        <f>IF(F26=E26+D26,0,1)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H26">
-        <f>IF(G26+F26&lt;E26+D26,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3793,27 +3822,27 @@
       <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D27">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B27,INPUT!$B:$B,"M")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B27,INPUT!$B:$B,"F")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <f>IF(AND(D27&lt;&gt;0, E27&lt;&gt;0),3,IF(D27+E27&gt;1,2,D27+E27))</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="G27">
-        <f>IF(F27=E27+D27,0,1)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H27">
-        <f>IF(G27+F27&lt;E27+D27,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3825,7 +3854,7 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D28">
@@ -3837,15 +3866,15 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <f>IF(AND(D28&lt;&gt;0, E28&lt;&gt;0),3,IF(D28+E28&gt;1,2,D28+E28))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G28">
-        <f>IF(F28=E28+D28,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28">
-        <f>IF(G28+F28&lt;E28+D28,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3857,7 +3886,7 @@
       <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D29">
@@ -3869,15 +3898,15 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <f>IF(AND(D29&lt;&gt;0, E29&lt;&gt;0),3,IF(D29+E29&gt;1,2,D29+E29))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G29">
-        <f>IF(F29=E29+D29,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H29">
-        <f>IF(G29+F29&lt;E29+D29,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3889,7 +3918,7 @@
       <c r="B30" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D30">
@@ -3901,15 +3930,15 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <f>IF(AND(D30&lt;&gt;0, E30&lt;&gt;0),3,IF(D30+E30&gt;1,2,D30+E30))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G30">
-        <f>IF(F30=E30+D30,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H30">
-        <f>IF(G30+F30&lt;E30+D30,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3921,7 +3950,7 @@
       <c r="B31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D31">
@@ -3933,15 +3962,15 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f>IF(AND(D31&lt;&gt;0, E31&lt;&gt;0),3,IF(D31+E31&gt;1,2,D31+E31))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G31">
-        <f>IF(F31=E31+D31,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H31">
-        <f>IF(G31+F31&lt;E31+D31,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3953,27 +3982,27 @@
       <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D32">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B32,INPUT!$B:$B,"M")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B32,INPUT!$B:$B,"F")</f>
         <v>0</v>
       </c>
       <c r="F32">
-        <f>IF(AND(D32&lt;&gt;0, E32&lt;&gt;0),3,IF(D32+E32&gt;1,2,D32+E32))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G32">
-        <f>IF(F32=E32+D32,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H32">
-        <f>IF(G32+F32&lt;E32+D32,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3985,7 +4014,7 @@
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D33">
@@ -3997,15 +4026,15 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <f>IF(AND(D33&lt;&gt;0, E33&lt;&gt;0),3,IF(D33+E33&gt;1,2,D33+E33))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G33">
-        <f>IF(F33=E33+D33,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H33">
-        <f>IF(G33+F33&lt;E33+D33,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4017,7 +4046,7 @@
       <c r="B34" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D34">
@@ -4029,15 +4058,15 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <f>IF(AND(D34&lt;&gt;0, E34&lt;&gt;0),3,IF(D34+E34&gt;1,2,D34+E34))</f>
+        <f t="shared" ref="F34:F65" si="3">IF(AND(D34&lt;&gt;0, E34&lt;&gt;0),3,IF(D34+E34&gt;1,2,D34+E34))</f>
         <v>1</v>
       </c>
       <c r="G34">
-        <f>IF(F34=E34+D34,0,1)</f>
+        <f t="shared" ref="G34:G65" si="4">IF(F34=E34+D34,0,1)</f>
         <v>0</v>
       </c>
       <c r="H34">
-        <f>IF(G34+F34&lt;E34+D34,1,0)</f>
+        <f t="shared" ref="H34:H65" si="5">IF(G34+F34&lt;E34+D34,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4049,7 +4078,7 @@
       <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D35">
@@ -4061,15 +4090,15 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <f>IF(AND(D35&lt;&gt;0, E35&lt;&gt;0),3,IF(D35+E35&gt;1,2,D35+E35))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G35">
-        <f>IF(F35=E35+D35,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H35">
-        <f>IF(G35+F35&lt;E35+D35,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4081,7 +4110,7 @@
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D36">
@@ -4093,15 +4122,15 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <f>IF(AND(D36&lt;&gt;0, E36&lt;&gt;0),3,IF(D36+E36&gt;1,2,D36+E36))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G36">
-        <f>IF(F36=E36+D36,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H36">
-        <f>IF(G36+F36&lt;E36+D36,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4121,15 +4150,15 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <f>IF(AND(D37&lt;&gt;0, E37&lt;&gt;0),3,IF(D37+E37&gt;1,2,D37+E37))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G37">
-        <f>IF(F37=E37+D37,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f>IF(G37+F37&lt;E37+D37,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4141,7 +4170,7 @@
       <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D38">
@@ -4153,15 +4182,15 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <f>IF(AND(D38&lt;&gt;0, E38&lt;&gt;0),3,IF(D38+E38&gt;1,2,D38+E38))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G38">
-        <f>IF(F38=E38+D38,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H38">
-        <f>IF(G38+F38&lt;E38+D38,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4173,7 +4202,7 @@
       <c r="B39" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D39">
@@ -4185,15 +4214,15 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <f>IF(AND(D39&lt;&gt;0, E39&lt;&gt;0),3,IF(D39+E39&gt;1,2,D39+E39))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G39">
-        <f>IF(F39=E39+D39,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H39">
-        <f>IF(G39+F39&lt;E39+D39,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4205,7 +4234,7 @@
       <c r="B40" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D40">
@@ -4217,15 +4246,15 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <f>IF(AND(D40&lt;&gt;0, E40&lt;&gt;0),3,IF(D40+E40&gt;1,2,D40+E40))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G40">
-        <f>IF(F40=E40+D40,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H40">
-        <f>IF(G40+F40&lt;E40+D40,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4245,15 +4274,15 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <f>IF(AND(D41&lt;&gt;0, E41&lt;&gt;0),3,IF(D41+E41&gt;1,2,D41+E41))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G41">
-        <f>IF(F41=E41+D41,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H41">
-        <f>IF(G41+F41&lt;E41+D41,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4273,15 +4302,15 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <f>IF(AND(D42&lt;&gt;0, E42&lt;&gt;0),3,IF(D42+E42&gt;1,2,D42+E42))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G42">
-        <f>IF(F42=E42+D42,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H42">
-        <f>IF(G42+F42&lt;E42+D42,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4301,15 +4330,15 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <f>IF(AND(D43&lt;&gt;0, E43&lt;&gt;0),3,IF(D43+E43&gt;1,2,D43+E43))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G43">
-        <f>IF(F43=E43+D43,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H43">
-        <f>IF(G43+F43&lt;E43+D43,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4329,15 +4358,15 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <f>IF(AND(D44&lt;&gt;0, E44&lt;&gt;0),3,IF(D44+E44&gt;1,2,D44+E44))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G44">
-        <f>IF(F44=E44+D44,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H44">
-        <f>IF(G44+F44&lt;E44+D44,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4357,15 +4386,15 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <f>IF(AND(D45&lt;&gt;0, E45&lt;&gt;0),3,IF(D45+E45&gt;1,2,D45+E45))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G45">
-        <f>IF(F45=E45+D45,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H45">
-        <f>IF(G45+F45&lt;E45+D45,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4385,15 +4414,15 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <f>IF(AND(D46&lt;&gt;0, E46&lt;&gt;0),3,IF(D46+E46&gt;1,2,D46+E46))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G46">
-        <f>IF(F46=E46+D46,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H46">
-        <f>IF(G46+F46&lt;E46+D46,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4413,15 +4442,15 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <f>IF(AND(D47&lt;&gt;0, E47&lt;&gt;0),3,IF(D47+E47&gt;1,2,D47+E47))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G47">
-        <f>IF(F47=E47+D47,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H47">
-        <f>IF(G47+F47&lt;E47+D47,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4441,15 +4470,15 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <f>IF(AND(D48&lt;&gt;0, E48&lt;&gt;0),3,IF(D48+E48&gt;1,2,D48+E48))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G48">
-        <f>IF(F48=E48+D48,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H48">
-        <f>IF(G48+F48&lt;E48+D48,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4469,15 +4498,15 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <f>IF(AND(D49&lt;&gt;0, E49&lt;&gt;0),3,IF(D49+E49&gt;1,2,D49+E49))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G49">
-        <f>IF(F49=E49+D49,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H49">
-        <f>IF(G49+F49&lt;E49+D49,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4489,7 +4518,7 @@
       <c r="B50" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D50">
@@ -4501,15 +4530,15 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <f>IF(AND(D50&lt;&gt;0, E50&lt;&gt;0),3,IF(D50+E50&gt;1,2,D50+E50))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G50">
-        <f>IF(F50=E50+D50,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H50">
-        <f>IF(G50+F50&lt;E50+D50,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4529,15 +4558,15 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <f>IF(AND(D51&lt;&gt;0, E51&lt;&gt;0),3,IF(D51+E51&gt;1,2,D51+E51))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G51">
-        <f>IF(F51=E51+D51,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H51">
-        <f>IF(G51+F51&lt;E51+D51,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4549,27 +4578,27 @@
       <c r="B52" t="s">
         <v>24</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="D52">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B52,INPUT!$B:$B,"M")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
         <f>COUNTIFS(INPUT!$A:$A,OUTPUT!$B52,INPUT!$B:$B,"F")</f>
         <v>0</v>
       </c>
       <c r="F52">
-        <f>IF(AND(D52&lt;&gt;0, E52&lt;&gt;0),3,IF(D52+E52&gt;1,2,D52+E52))</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="G52">
-        <f>IF(F52=E52+D52,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H52">
-        <f>IF(G52+F52&lt;E52+D52,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4581,7 +4610,7 @@
       <c r="B53" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D53">
@@ -4593,15 +4622,15 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <f>IF(AND(D53&lt;&gt;0, E53&lt;&gt;0),3,IF(D53+E53&gt;1,2,D53+E53))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G53">
-        <f>IF(F53=E53+D53,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H53">
-        <f>IF(G53+F53&lt;E53+D53,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4621,15 +4650,15 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <f>IF(AND(D54&lt;&gt;0, E54&lt;&gt;0),3,IF(D54+E54&gt;1,2,D54+E54))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G54">
-        <f>IF(F54=E54+D54,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H54">
-        <f>IF(G54+F54&lt;E54+D54,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4649,15 +4678,15 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <f>IF(AND(D55&lt;&gt;0, E55&lt;&gt;0),3,IF(D55+E55&gt;1,2,D55+E55))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G55">
-        <f>IF(F55=E55+D55,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H55">
-        <f>IF(G55+F55&lt;E55+D55,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4677,15 +4706,15 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <f>IF(AND(D56&lt;&gt;0, E56&lt;&gt;0),3,IF(D56+E56&gt;1,2,D56+E56))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G56">
-        <f>IF(F56=E56+D56,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H56">
-        <f>IF(G56+F56&lt;E56+D56,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4705,15 +4734,15 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <f>IF(AND(D57&lt;&gt;0, E57&lt;&gt;0),3,IF(D57+E57&gt;1,2,D57+E57))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G57">
-        <f>IF(F57=E57+D57,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H57">
-        <f>IF(G57+F57&lt;E57+D57,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4733,15 +4762,15 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <f>IF(AND(D58&lt;&gt;0, E58&lt;&gt;0),3,IF(D58+E58&gt;1,2,D58+E58))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G58">
-        <f>IF(F58=E58+D58,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H58">
-        <f>IF(G58+F58&lt;E58+D58,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4761,15 +4790,15 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <f>IF(AND(D59&lt;&gt;0, E59&lt;&gt;0),3,IF(D59+E59&gt;1,2,D59+E59))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G59">
-        <f>IF(F59=E59+D59,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H59">
-        <f>IF(G59+F59&lt;E59+D59,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4781,7 +4810,7 @@
       <c r="B60" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D60">
@@ -4793,15 +4822,15 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <f>IF(AND(D60&lt;&gt;0, E60&lt;&gt;0),3,IF(D60+E60&gt;1,2,D60+E60))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G60">
-        <f>IF(F60=E60+D60,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H60">
-        <f>IF(G60+F60&lt;E60+D60,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4821,15 +4850,15 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <f>IF(AND(D61&lt;&gt;0, E61&lt;&gt;0),3,IF(D61+E61&gt;1,2,D61+E61))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G61">
-        <f>IF(F61=E61+D61,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H61">
-        <f>IF(G61+F61&lt;E61+D61,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4841,7 +4870,7 @@
       <c r="B62" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D62">
@@ -4853,15 +4882,15 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <f>IF(AND(D62&lt;&gt;0, E62&lt;&gt;0),3,IF(D62+E62&gt;1,2,D62+E62))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G62">
-        <f>IF(F62=E62+D62,0,1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H62">
-        <f>IF(G62+F62&lt;E62+D62,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4881,15 +4910,15 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <f>IF(AND(D63&lt;&gt;0, E63&lt;&gt;0),3,IF(D63+E63&gt;1,2,D63+E63))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G63">
-        <f>IF(F63=E63+D63,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H63">
-        <f>IF(G63+F63&lt;E63+D63,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4909,15 +4938,15 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <f>IF(AND(D64&lt;&gt;0, E64&lt;&gt;0),3,IF(D64+E64&gt;1,2,D64+E64))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G64">
-        <f>IF(F64=E64+D64,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H64">
-        <f>IF(G64+F64&lt;E64+D64,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4937,15 +4966,15 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <f>IF(AND(D65&lt;&gt;0, E65&lt;&gt;0),3,IF(D65+E65&gt;1,2,D65+E65))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G65">
-        <f>IF(F65=E65+D65,0,1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H65">
-        <f>IF(G65+F65&lt;E65+D65,1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4965,15 +4994,15 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <f>IF(AND(D66&lt;&gt;0, E66&lt;&gt;0),3,IF(D66+E66&gt;1,2,D66+E66))</f>
+        <f t="shared" ref="F66:F97" si="6">IF(AND(D66&lt;&gt;0, E66&lt;&gt;0),3,IF(D66+E66&gt;1,2,D66+E66))</f>
         <v>0</v>
       </c>
       <c r="G66">
-        <f>IF(F66=E66+D66,0,1)</f>
+        <f t="shared" ref="G66:G97" si="7">IF(F66=E66+D66,0,1)</f>
         <v>0</v>
       </c>
       <c r="H66">
-        <f>IF(G66+F66&lt;E66+D66,1,0)</f>
+        <f t="shared" ref="H66:H97" si="8">IF(G66+F66&lt;E66+D66,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4993,15 +5022,15 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <f>IF(AND(D67&lt;&gt;0, E67&lt;&gt;0),3,IF(D67+E67&gt;1,2,D67+E67))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G67">
-        <f>IF(F67=E67+D67,0,1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H67">
-        <f>IF(G67+F67&lt;E67+D67,1,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5021,15 +5050,15 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <f>IF(AND(D68&lt;&gt;0, E68&lt;&gt;0),3,IF(D68+E68&gt;1,2,D68+E68))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G68">
-        <f>IF(F68=E68+D68,0,1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H68">
-        <f>IF(G68+F68&lt;E68+D68,1,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5049,15 +5078,15 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <f>IF(AND(D69&lt;&gt;0, E69&lt;&gt;0),3,IF(D69+E69&gt;1,2,D69+E69))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G69">
-        <f>IF(F69=E69+D69,0,1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H69">
-        <f>IF(G69+F69&lt;E69+D69,1,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5069,7 +5098,7 @@
       <c r="B70" t="s">
         <v>42</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D70">
@@ -5081,15 +5110,15 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <f>IF(AND(D70&lt;&gt;0, E70&lt;&gt;0),3,IF(D70+E70&gt;1,2,D70+E70))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G70">
-        <f>IF(F70=E70+D70,0,1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H70">
-        <f>IF(G70+F70&lt;E70+D70,1,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5103,7 +5132,7 @@
       </c>
       <c r="G71">
         <f>SUM(G2:G70)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H71">
         <f>SUM(H2:H70)</f>
@@ -5116,7 +5145,7 @@
       </c>
       <c r="H72">
         <f>SUM(F71:I71)</f>
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>